<commit_message>
Atualização do arquivo CondominioDosIpes e otimização do powerflow
</commit_message>
<xml_diff>
--- a/data/spreadsheets/sheet_5Node.xlsx
+++ b/data/spreadsheets/sheet_5Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37606F46-7BD8-4C56-A23F-5769A2E3C3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE1580C-E489-44A2-A358-7FBFFFDD056B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13224" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="63">
   <si>
     <t>Parameter</t>
   </si>
@@ -147,9 +147,6 @@
     <t>MAC003998.csv</t>
   </si>
   <si>
-    <t>pub_ilum</t>
-  </si>
-  <si>
     <t>0.9823</t>
   </si>
   <si>
@@ -184,6 +181,51 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>MAC004000.csv</t>
+  </si>
+  <si>
+    <t>MAC004000</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>bus_001</t>
+  </si>
+  <si>
+    <t>bus_002</t>
+  </si>
+  <si>
+    <t>bus_003</t>
+  </si>
+  <si>
+    <t>bus_004</t>
+  </si>
+  <si>
+    <t>bus_005</t>
+  </si>
+  <si>
+    <t>bus_006</t>
+  </si>
+  <si>
+    <t>ip_001</t>
+  </si>
+  <si>
+    <t>ip_002</t>
+  </si>
+  <si>
+    <t>ip_003</t>
+  </si>
+  <si>
+    <t>ip_004</t>
+  </si>
+  <si>
+    <t>ip_005</t>
+  </si>
+  <si>
+    <t>ip_006</t>
   </si>
 </sst>
 </file>
@@ -585,7 +627,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -622,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41462.270833333336</v>
+        <v>41098.270833333336</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>20</v>
@@ -661,10 +703,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -673,7 +715,7 @@
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
@@ -683,66 +725,78 @@
       <c r="C1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="K1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>4</v>
+      <c r="B2" t="s">
+        <v>51</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>10</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2">
+        <v>123</v>
+      </c>
+      <c r="H2" s="5">
         <v>50</v>
       </c>
-      <c r="G2" s="5">
+      <c r="I2" s="5">
         <v>30</v>
       </c>
-      <c r="H2" s="16">
+      <c r="J2" s="16">
         <v>10</v>
       </c>
-      <c r="I2" s="16">
+      <c r="K2" s="16">
         <v>90</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="11"/>
       <c r="H3" s="17"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
     </row>
   </sheetData>
@@ -759,7 +813,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -803,8 +857,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>51</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -825,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="2">
         <v>123</v>
@@ -867,7 +921,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -916,10 +970,10 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -934,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -946,7 +1000,7 @@
         <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
         <v>29</v>
@@ -954,10 +1008,10 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -984,7 +1038,7 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
@@ -992,10 +1046,10 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1022,7 +1076,7 @@
         <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L4" t="s">
         <v>31</v>
@@ -1030,10 +1084,10 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1060,7 +1114,7 @@
         <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L5" t="s">
         <v>32</v>
@@ -1068,10 +1122,10 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1098,10 +1152,48 @@
         <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L6" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1121,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3425D832-8626-4E16-B86F-D606408C1A89}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1171,17 +1263,17 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="A2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1190,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -1205,21 +1297,21 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="A3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -1228,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3">
         <v>8</v>
@@ -1243,21 +1335,21 @@
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="A4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -1266,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -1281,21 +1373,21 @@
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="A5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -1304,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5">
         <v>8</v>
@@ -1319,21 +1411,21 @@
         <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+      <c r="A6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -1342,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <v>8</v>
@@ -1357,11 +1449,46 @@
         <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K7" s="19"/>
+      <c r="A7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="19">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K8" s="19"/>

</xml_diff>

<commit_message>
Correção de algumas funções e ajuste para rodar o fluxo novamente
</commit_message>
<xml_diff>
--- a/data/spreadsheets/sheet_5Node.xlsx
+++ b/data/spreadsheets/sheet_5Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE1580C-E489-44A2-A358-7FBFFFDD056B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9270C2B8-E80C-4FE4-BF00-00F77A4915D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13224" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
   <si>
     <t>Parameter</t>
   </si>
@@ -183,15 +183,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>MAC004000.csv</t>
-  </si>
-  <si>
-    <t>MAC004000</t>
-  </si>
-  <si>
-    <t>0.96</t>
-  </si>
-  <si>
     <t>bus_001</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
     <t>bus_005</t>
   </si>
   <si>
-    <t>bus_006</t>
-  </si>
-  <si>
     <t>ip_001</t>
   </si>
   <si>
@@ -223,9 +211,6 @@
   </si>
   <si>
     <t>ip_005</t>
-  </si>
-  <si>
-    <t>ip_006</t>
   </si>
 </sst>
 </file>
@@ -627,7 +612,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -664,7 +649,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41098.270833333336</v>
+        <v>41098.25</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>20</v>
@@ -758,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -858,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -921,7 +906,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -973,7 +958,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1011,7 +996,7 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1049,7 +1034,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1087,7 +1072,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1125,7 +1110,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1156,44 +1141,6 @@
       </c>
       <c r="L6" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3425D832-8626-4E16-B86F-D606408C1A89}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1264,10 +1211,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1302,10 +1249,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1340,10 +1287,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1378,10 +1325,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1416,10 +1363,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1453,42 +1400,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="19">
-        <v>13</v>
-      </c>
-      <c r="L7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A7" s="11"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K8" s="19"/>

</xml_diff>

<commit_message>
Fluxo de potência correto
</commit_message>
<xml_diff>
--- a/data/spreadsheets/sheet_5Node.xlsx
+++ b/data/spreadsheets/sheet_5Node.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Code\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9270C2B8-E80C-4FE4-BF00-00F77A4915D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2007DB-DF91-4B1E-BE2B-DE5426F17B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -613,7 +613,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41098.25</v>
+        <v>41462.25</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>20</v>

</xml_diff>